<commit_message>
add message queue for temperature
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="59">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -177,6 +177,21 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;value&gt; °</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResourceId1</t>
   </si>
 </sst>
 </file>
@@ -1656,7 +1671,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -1668,6 +1683,23 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Start and Develop buttons to the UI
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="64">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -192,6 +192,21 @@
   </si>
   <si>
     <t xml:space="preserve">ResourceId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
   </si>
 </sst>
 </file>
@@ -1703,6 +1718,41 @@
         <v>49</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>